<commit_message>
Fix onboarding state logic
</commit_message>
<xml_diff>
--- a/server/database.xlsx
+++ b/server/database.xlsx
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -415,58 +415,75 @@
         <v>completed</v>
       </c>
       <c r="D1" t="str">
+        <v>priority</v>
+      </c>
+      <c r="E1" t="str">
+        <v>createdAt</v>
+      </c>
+      <c r="F1" t="str">
         <v>dueDate</v>
-      </c>
-      <c r="E1" t="str">
-        <v>priority</v>
-      </c>
-      <c r="F1" t="str">
-        <v>createdAt</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>e57c802d-7533-4e70-8e72-c92506dd43e8</v>
+        <v>00037519-1bcb-4bb8-b2e0-1dff1cb4eb99</v>
       </c>
       <c r="B2" t="str">
-        <v>ds c nc d</v>
+        <v>jnvjdnvds</v>
       </c>
       <c r="C2" t="b">
         <v>0</v>
       </c>
       <c r="D2" t="str">
-        <v>2025-11-22</v>
-      </c>
-      <c r="E2" t="str">
         <v>medium</v>
       </c>
-      <c r="F2">
-        <v>1763734626268</v>
+      <c r="E2">
+        <v>1763735225324</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>a3c0ba97-0e64-4167-863b-4892b84ce151</v>
+        <v>e57c802d-7533-4e70-8e72-c92506dd43e8</v>
       </c>
       <c r="B3" t="str">
-        <v>q</v>
+        <v>ds c nc d</v>
       </c>
       <c r="C3" t="b">
         <v>0</v>
       </c>
       <c r="D3" t="str">
+        <v>medium</v>
+      </c>
+      <c r="E3">
+        <v>1763734626268</v>
+      </c>
+      <c r="F3" t="str">
+        <v>2025-11-22</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>a3c0ba97-0e64-4167-863b-4892b84ce151</v>
+      </c>
+      <c r="B4" t="str">
+        <v>q</v>
+      </c>
+      <c r="C4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" t="str">
+        <v>medium</v>
+      </c>
+      <c r="E4">
+        <v>1763733656091</v>
+      </c>
+      <c r="F4" t="str">
         <v>2025-11-15</v>
-      </c>
-      <c r="E3" t="str">
-        <v>medium</v>
-      </c>
-      <c r="F3">
-        <v>1763733656091</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F4"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Fix finance category dropdown selection
</commit_message>
<xml_diff>
--- a/server/database.xlsx
+++ b/server/database.xlsx
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -426,10 +426,10 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>00037519-1bcb-4bb8-b2e0-1dff1cb4eb99</v>
+        <v>a3c0ba97-0e64-4167-863b-4892b84ce151</v>
       </c>
       <c r="B2" t="str">
-        <v>jnvjdnvds</v>
+        <v>q</v>
       </c>
       <c r="C2" t="b">
         <v>0</v>
@@ -438,52 +438,15 @@
         <v>medium</v>
       </c>
       <c r="E2">
-        <v>1763735225324</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>e57c802d-7533-4e70-8e72-c92506dd43e8</v>
-      </c>
-      <c r="B3" t="str">
-        <v>ds c nc d</v>
-      </c>
-      <c r="C3" t="b">
-        <v>0</v>
-      </c>
-      <c r="D3" t="str">
-        <v>medium</v>
-      </c>
-      <c r="E3">
-        <v>1763734626268</v>
-      </c>
-      <c r="F3" t="str">
-        <v>2025-11-22</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>a3c0ba97-0e64-4167-863b-4892b84ce151</v>
-      </c>
-      <c r="B4" t="str">
-        <v>q</v>
-      </c>
-      <c r="C4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D4" t="str">
-        <v>medium</v>
-      </c>
-      <c r="E4">
         <v>1763733656091</v>
       </c>
-      <c r="F4" t="str">
+      <c r="F2" t="str">
         <v>2025-11-15</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F2"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>